<commit_message>
Added words from Benefit report
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bgebert/Scripts/SHRM/get_workle_words/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700F7A30-7F0C-9941-B89B-4971353477DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B65C1F-1A7D-7C47-8C4F-18AA7E0FBA29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="2100" windowWidth="27240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38420" yWindow="500" windowWidth="27240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="glossary_template" sheetId="1" r:id="rId1"/>
     <sheet name="Unused" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">glossary_template!$A$1:$M$118</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -343,7 +346,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="318">
   <si>
     <t>GLOSSARY</t>
   </si>
@@ -1267,6 +1270,36 @@
   </si>
   <si>
     <t>Total Length</t>
+  </si>
+  <si>
+    <t>https://shrm.org/benefits</t>
+  </si>
+  <si>
+    <t>flex work</t>
+  </si>
+  <si>
+    <t>BENEFITS</t>
+  </si>
+  <si>
+    <t>63% of organizations said they offered some type of hybrid work opportunities in 2022. Additionally, 62% said they offer those employees with some type of subsidy or reimbursement for at home office or work equipment. Visit shrm.org/benefits to discover how your organization compares to others across flexible work and other types of benefits.</t>
+  </si>
+  <si>
+    <t>savings</t>
+  </si>
+  <si>
+    <t>In 2022, employers ranked retirement and savings benefits as among the most important types they can offer to employees. Most employers offered some type of retirement savings plan to their employees. Visit shrm.org/benefits to explore more retirement and savings benefits trends.</t>
+  </si>
+  <si>
+    <t>tuition</t>
+  </si>
+  <si>
+    <t>Nearly half of organizations (48%) offer undergraduate or graduate tuition assistance as an employee benefit. There are many other ways in which organizations use benefits to support their employees’ professional development and growth. Visit shrm.org/benefits to discover how your organization compares to others across these and other types of benefits.</t>
+  </si>
+  <si>
+    <t>program</t>
+  </si>
+  <si>
+    <t>Employers can offer several types of programs that focus of health and wellbeing as an employee benefit. These programs can include weight loss, tobacco cessation, and general wellness programs covering many health-related areas. Visit shrm.org/benefits to discover how your organization compares to others across these and other types of benefits.</t>
   </si>
 </sst>
 </file>
@@ -1873,7 +1906,43 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="133">
+  <dxfs count="136">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -3782,8 +3851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3842,7 +3911,7 @@
       </c>
       <c r="E2" s="1">
         <f ca="1">RAND()</f>
-        <v>0.64635542535944668</v>
+        <v>0.96360257642576097</v>
       </c>
       <c r="F2" s="1">
         <f>IF(ISNUMBER(SEARCH(" ",D2)), LEN(LEFT(D2,FIND(" ",D2)-1)), LEN(D2))</f>
@@ -3878,7 +3947,7 @@
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E93" ca="1" si="2">RAND()</f>
-        <v>0.84119176337953694</v>
+        <v>0.13654140152476824</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" ref="F3:F17" si="3">IF(ISNUMBER(SEARCH(" ",D3)), LEN(LEFT(D3,FIND(" ",D3)-1)), LEN(D3))</f>
@@ -3914,7 +3983,7 @@
       </c>
       <c r="E4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>2.7780392313871083E-2</v>
+        <v>0.81831547861562137</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="3"/>
@@ -3950,7 +4019,7 @@
       </c>
       <c r="E5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86655697838007351</v>
+        <v>0.75215034146211246</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="3"/>
@@ -3986,7 +4055,7 @@
       </c>
       <c r="E6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.64607076478085645</v>
+        <v>0.29396968462057871</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="3"/>
@@ -4022,7 +4091,7 @@
       </c>
       <c r="E7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.45070883362861158</v>
+        <v>0.33254610003423501</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="3"/>
@@ -4058,7 +4127,7 @@
       </c>
       <c r="E8" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>7.0443150660142617E-2</v>
+        <v>0.76876129079304212</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="3"/>
@@ -4094,7 +4163,7 @@
       </c>
       <c r="E9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.30711236773742223</v>
+        <v>0.75035905144304471</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="3"/>
@@ -4130,7 +4199,7 @@
       </c>
       <c r="E10" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.60841520956455153</v>
+        <v>0.83559027041126832</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="3"/>
@@ -4166,7 +4235,7 @@
       </c>
       <c r="E11" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.34166024552033369</v>
+        <v>0.6518943267385332</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="3"/>
@@ -4202,7 +4271,7 @@
       </c>
       <c r="E12" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.49197341307466802</v>
+        <v>0.27688329289420566</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="3"/>
@@ -4238,7 +4307,7 @@
       </c>
       <c r="E13" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.77058038616394531</v>
+        <v>0.4103028224971691</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="3"/>
@@ -4274,7 +4343,7 @@
       </c>
       <c r="E14" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.90316738253937878</v>
+        <v>0.54754063057386204</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="3"/>
@@ -4310,7 +4379,7 @@
       </c>
       <c r="E15" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.76475449831736397</v>
+        <v>0.11164690948571554</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="3"/>
@@ -4346,7 +4415,7 @@
       </c>
       <c r="E16" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.76647441512847725</v>
+        <v>0.53800138363370975</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="3"/>
@@ -4382,7 +4451,7 @@
       </c>
       <c r="E17" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85260130228169551</v>
+        <v>0.50629914868341608</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="3"/>
@@ -4418,7 +4487,7 @@
       </c>
       <c r="E18" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.7894852495486625</v>
+        <v>8.9775795340380604E-2</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" ref="F18:F78" si="7">IF(ISNUMBER(SEARCH(" ",D18)), LEN(LEFT(D18,FIND(" ",D18)-1)), LEN(D18))</f>
@@ -4454,7 +4523,7 @@
       </c>
       <c r="E19" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.98111648947295382</v>
+        <v>0.65843705336380065</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="7"/>
@@ -4493,7 +4562,7 @@
       </c>
       <c r="E20" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.97392718509078013</v>
+        <v>3.7818841890921551E-2</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="7"/>
@@ -4529,7 +4598,7 @@
       </c>
       <c r="E21" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.17070365343943283</v>
+        <v>0.10827122149326174</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="7"/>
@@ -4565,7 +4634,7 @@
       </c>
       <c r="E22" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.11030760611326196</v>
+        <v>0.63708543595859357</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="7"/>
@@ -4601,7 +4670,7 @@
       </c>
       <c r="E23" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.75575962227435034</v>
+        <v>0.26810728794592498</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="7"/>
@@ -4637,7 +4706,7 @@
       </c>
       <c r="E24" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.51921167816750624</v>
+        <v>0.32281333881673668</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" si="7"/>
@@ -4673,7 +4742,7 @@
       </c>
       <c r="E25" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.36174158854309513</v>
+        <v>0.48566444374424544</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" si="7"/>
@@ -4709,7 +4778,7 @@
       </c>
       <c r="E26" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.6144192798946696</v>
+        <v>0.83557099968033199</v>
       </c>
       <c r="F26" s="1">
         <f t="shared" si="7"/>
@@ -4745,7 +4814,7 @@
       </c>
       <c r="E27" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.37564015340955781</v>
+        <v>0.54909284137632075</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" si="7"/>
@@ -4781,7 +4850,7 @@
       </c>
       <c r="E28" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.75402571418256104</v>
+        <v>0.54084321772022115</v>
       </c>
       <c r="F28" s="1">
         <f t="shared" si="7"/>
@@ -4817,7 +4886,7 @@
       </c>
       <c r="E29" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.98939694996243022</v>
+        <v>0.15436178273881807</v>
       </c>
       <c r="F29" s="1">
         <f t="shared" si="7"/>
@@ -4853,7 +4922,7 @@
       </c>
       <c r="E30" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.39788425347557566</v>
+        <v>0.75090116973128984</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" si="7"/>
@@ -4892,7 +4961,7 @@
       </c>
       <c r="E31" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.46864028530247259</v>
+        <v>1.2639390187181299E-2</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" si="7"/>
@@ -4937,7 +5006,7 @@
       </c>
       <c r="E32" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>7.7140515222744344E-2</v>
+        <v>7.8473881022594227E-2</v>
       </c>
       <c r="F32" s="1">
         <f t="shared" si="7"/>
@@ -4968,7 +5037,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>93</v>
+        <v>310</v>
       </c>
       <c r="B33" s="2">
         <v>44681</v>
@@ -4982,7 +5051,7 @@
       </c>
       <c r="E33" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.77573518921661999</v>
+        <v>0.22524887346521738</v>
       </c>
       <c r="F33" s="1">
         <f t="shared" si="7"/>
@@ -5003,17 +5072,17 @@
       <c r="K33" t="s">
         <v>190</v>
       </c>
-      <c r="L33" t="s">
-        <v>187</v>
+      <c r="L33" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M33" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>,{"id":"18.6","date":"04/30/2022","word":"account","CLUE":"","factoid":"Many employers offer different types of savings accounts to employees as benefits, such as flexible spending accounts or health savings accounts. Check out how many offer these savings plans in SHRM's Employee Benefits Survey. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"18.6","date":"04/30/2022","word":"account","CLUE":"","factoid":"Many employers offer different types of savings accounts to employees as benefits, such as flexible spending accounts or health savings accounts. Check out how many offer these savings plans in SHRM's Employee Benefits Survey. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>93</v>
+        <v>310</v>
       </c>
       <c r="B34" s="2">
         <v>44682</v>
@@ -5027,7 +5096,7 @@
       </c>
       <c r="E34" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.68374869615981004</v>
+        <v>8.444742790919324E-2</v>
       </c>
       <c r="F34" s="1">
         <f t="shared" si="7"/>
@@ -5048,17 +5117,17 @@
       <c r="K34" t="s">
         <v>192</v>
       </c>
-      <c r="L34" t="s">
-        <v>187</v>
+      <c r="L34" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M34" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>,{"id":"19.0","date":"05/01/2022","word":"dental","CLUE":"","factoid":"98% of organizations offer dental insurance as an employee benefit in 2022. But there are many other benefits employees might offer to take care of their employees. Check out results from SHRM's Employee Benefits Survey to see how many of these benefits are offered by others. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"19.0","date":"05/01/2022","word":"dental","CLUE":"","factoid":"98% of organizations offer dental insurance as an employee benefit in 2022. But there are many other benefits employees might offer to take care of their employees. Check out results from SHRM's Employee Benefits Survey to see how many of these benefits are offered by others. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>93</v>
+        <v>310</v>
       </c>
       <c r="B35" s="2">
         <v>44683</v>
@@ -5072,7 +5141,7 @@
       </c>
       <c r="E35" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.31139312995808011</v>
+        <v>0.50581067669324986</v>
       </c>
       <c r="F35" s="1">
         <f t="shared" si="7"/>
@@ -5093,17 +5162,17 @@
       <c r="K35" t="s">
         <v>193</v>
       </c>
-      <c r="L35" t="s">
-        <v>187</v>
+      <c r="L35" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M35" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>,{"id":"19.1","date":"05/02/2022","word":"vision ","CLUE":"","factoid":"94% of organizations offer vision insurance as an employee benefit in 2022. But there are many other benefits employees might offer to take care of their employees. Check out results from SHRM's Employee Benefits Survey to see how many of these benefits are offered by others. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"19.1","date":"05/02/2022","word":"vision ","CLUE":"","factoid":"94% of organizations offer vision insurance as an employee benefit in 2022. But there are many other benefits employees might offer to take care of their employees. Check out results from SHRM's Employee Benefits Survey to see how many of these benefits are offered by others. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>93</v>
+        <v>310</v>
       </c>
       <c r="B36" s="2">
         <v>44684</v>
@@ -5117,7 +5186,7 @@
       </c>
       <c r="E36" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.24037779786057845</v>
+        <v>7.3773252337925088E-2</v>
       </c>
       <c r="F36" s="1">
         <f t="shared" si="7"/>
@@ -5138,17 +5207,17 @@
       <c r="K36" t="s">
         <v>194</v>
       </c>
-      <c r="L36" t="s">
-        <v>187</v>
+      <c r="L36" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M36" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>,{"id":"19.2","date":"05/03/2022","word":"health","CLUE":"","factoid":"Benefits focusing on employee health are a great tool employers can use to attract the best talent but more importantly, to keep their employees safe. Check out SHRM's Employee Benefits Survey to see which health-related benefits were among those most often offered. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"19.2","date":"05/03/2022","word":"health","CLUE":"","factoid":"Benefits focusing on employee health are a great tool employers can use to attract the best talent but more importantly, to keep their employees safe. Check out SHRM's Employee Benefits Survey to see which health-related benefits were among those most often offered. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>93</v>
+        <v>310</v>
       </c>
       <c r="B37" s="2">
         <v>44685</v>
@@ -5162,7 +5231,7 @@
       </c>
       <c r="E37" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.66317482530159078</v>
+        <v>0.9002640781607183</v>
       </c>
       <c r="F37" s="1">
         <f t="shared" si="7"/>
@@ -5183,17 +5252,17 @@
       <c r="K37" t="s">
         <v>195</v>
       </c>
-      <c r="L37" t="s">
-        <v>187</v>
+      <c r="L37" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M37" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>,{"id":"19.3","date":"05/04/2022","word":"mental","CLUE":"","factoid":"More employers than ever offered employees mental health benefits in 2022 than ever before. See what other health and wellness benefits were offered in SHRM's Employee Benefits Survey. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"19.3","date":"05/04/2022","word":"mental","CLUE":"","factoid":"More employers than ever offered employees mental health benefits in 2022 than ever before. See what other health and wellness benefits were offered in SHRM's Employee Benefits Survey. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>93</v>
+        <v>310</v>
       </c>
       <c r="B38" s="2">
         <v>44686</v>
@@ -5207,7 +5276,7 @@
       </c>
       <c r="E38" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.1957228574420522</v>
+        <v>0.75124633977219035</v>
       </c>
       <c r="F38" s="1">
         <f t="shared" si="7"/>
@@ -5228,17 +5297,17 @@
       <c r="K38" t="s">
         <v>196</v>
       </c>
-      <c r="L38" t="s">
-        <v>187</v>
+      <c r="L38" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M38" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>,{"id":"19.4","date":"05/05/2022","word":"rewards","CLUE":"","factoid":"Offering employees rewards for participating in health and wellness programs is a great benefits you can offer to encourage employees to take care of themselves. See what other health and wellness beneifts were offered in SHRM's Employee Benefits Survey. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"19.4","date":"05/05/2022","word":"rewards","CLUE":"","factoid":"Offering employees rewards for participating in health and wellness programs is a great benefits you can offer to encourage employees to take care of themselves. See what other health and wellness beneifts were offered in SHRM's Employee Benefits Survey. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>93</v>
+        <v>310</v>
       </c>
       <c r="B39" s="2">
         <v>44687</v>
@@ -5252,7 +5321,7 @@
       </c>
       <c r="E39" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.73339371212009297</v>
+        <v>0.2584371638538302</v>
       </c>
       <c r="F39" s="1">
         <f t="shared" si="7"/>
@@ -5273,17 +5342,17 @@
       <c r="K39" t="s">
         <v>198</v>
       </c>
-      <c r="L39" t="s">
-        <v>187</v>
+      <c r="L39" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M39" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>,{"id":"19.5","date":"05/06/2022","word":"coach","CLUE":"","factoid":"Employers can provide access to various types of coaches or specialists as a benefit, such as nutritional or life coaching. Check out results from SHRM's Employee Benefits Survey to learn what types of benefits organizations are offering. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"19.5","date":"05/06/2022","word":"coach","CLUE":"","factoid":"Employers can provide access to various types of coaches or specialists as a benefit, such as nutritional or life coaching. Check out results from SHRM's Employee Benefits Survey to learn what types of benefits organizations are offering. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>94</v>
+        <v>310</v>
       </c>
       <c r="B40" s="2">
         <v>44688</v>
@@ -5297,7 +5366,7 @@
       </c>
       <c r="E40" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.79992580530058199</v>
+        <v>0.13361835612063633</v>
       </c>
       <c r="F40" s="1">
         <f t="shared" si="7"/>
@@ -5318,12 +5387,12 @@
       <c r="K40" t="s">
         <v>199</v>
       </c>
-      <c r="L40" t="s">
-        <v>187</v>
+      <c r="L40" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M40" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>,{"id":"19.6","date":"05/07/2022","word":"leave","CLUE":"","factoid":"Leave continues to be ranked among the most important types of benefits employers believe they can offer. Learn more about the types of leave and other benefits in SHRM's Employee Benefits Survey. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"19.6","date":"05/07/2022","word":"leave","CLUE":"","factoid":"Leave continues to be ranked among the most important types of benefits employers believe they can offer. Learn more about the types of leave and other benefits in SHRM's Employee Benefits Survey. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
@@ -5342,7 +5411,7 @@
       </c>
       <c r="E41" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.76077471138567387</v>
+        <v>0.28843093083469751</v>
       </c>
       <c r="F41" s="1">
         <f t="shared" si="7"/>
@@ -5373,7 +5442,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>94</v>
+        <v>310</v>
       </c>
       <c r="B42" s="2">
         <v>44690</v>
@@ -5387,7 +5456,7 @@
       </c>
       <c r="E42" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.97609669248544506</v>
+        <v>0.18944995655047414</v>
       </c>
       <c r="F42" s="1">
         <f t="shared" si="7"/>
@@ -5408,17 +5477,17 @@
       <c r="K42" t="s">
         <v>211</v>
       </c>
-      <c r="L42" t="s">
-        <v>187</v>
+      <c r="L42" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M42" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>,{"id":"20.1","date":"05/09/2022","word":"mentor","CLUE":"","factoid":"Mentorship programs are a great way in which employers can allow employees to connect and learn from each other. Find out how many organizations offered a mentorship program by visiting SHRM's Employee Benefits Survey. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"20.1","date":"05/09/2022","word":"mentor","CLUE":"","factoid":"Mentorship programs are a great way in which employers can allow employees to connect and learn from each other. Find out how many organizations offered a mentorship program by visiting SHRM's Employee Benefits Survey. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>93</v>
+        <v>310</v>
       </c>
       <c r="B43" s="2">
         <v>44691</v>
@@ -5432,7 +5501,7 @@
       </c>
       <c r="E43" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.81782757017040475</v>
+        <v>0.9224029664730008</v>
       </c>
       <c r="F43" s="1">
         <f t="shared" si="7"/>
@@ -5453,17 +5522,17 @@
       <c r="K43" t="s">
         <v>210</v>
       </c>
-      <c r="L43" t="s">
-        <v>187</v>
+      <c r="L43" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M43" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>,{"id":"20.2","date":"05/10/2022","word":"paycard","CLUE":"","factoid":"Paycards allow employers to provide employees with compensation by transfering funds to a debit card rather than to an employee's bank account. Find out how many offered this and other types of benefits by visiting SHRM's Employee Benefits Survey. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"20.2","date":"05/10/2022","word":"paycard","CLUE":"","factoid":"Paycards allow employers to provide employees with compensation by transfering funds to a debit card rather than to an employee's bank account. Find out how many offered this and other types of benefits by visiting SHRM's Employee Benefits Survey. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>93</v>
+        <v>310</v>
       </c>
       <c r="B44" s="2">
         <v>44692</v>
@@ -5477,7 +5546,7 @@
       </c>
       <c r="E44" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.59845148111292146</v>
+        <v>0.55284019872011181</v>
       </c>
       <c r="F44" s="1">
         <f t="shared" si="7"/>
@@ -5498,12 +5567,12 @@
       <c r="K44" t="s">
         <v>188</v>
       </c>
-      <c r="L44" t="s">
-        <v>187</v>
+      <c r="L44" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M44" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>,{"id":"20.3","date":"05/11/2022","word":"benefit","CLUE":"","factoid":"Non-wage forms of compensation offered to employees in exchange for work. While many organizations offer many of the same types of benefits, there are almost always differences between them. Check out SHRM's Employee Benefit Survey to see how many organizations offer different types of benefits. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"20.3","date":"05/11/2022","word":"benefit","CLUE":"","factoid":"Non-wage forms of compensation offered to employees in exchange for work. While many organizations offer many of the same types of benefits, there are almost always differences between them. Check out SHRM's Employee Benefit Survey to see how many organizations offer different types of benefits. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
@@ -5522,7 +5591,7 @@
       </c>
       <c r="E45" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.95707939979664947</v>
+        <v>4.2192135862707758E-2</v>
       </c>
       <c r="F45" s="1">
         <f t="shared" si="7"/>
@@ -5564,7 +5633,7 @@
       </c>
       <c r="E46" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.69801958220843208</v>
+        <v>0.63007411696403381</v>
       </c>
       <c r="F46" s="1">
         <f t="shared" si="7"/>
@@ -5606,7 +5675,7 @@
       </c>
       <c r="E47" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.18305495723083387</v>
+        <v>0.4462333332588988</v>
       </c>
       <c r="F47" s="1">
         <f t="shared" si="7"/>
@@ -5648,7 +5717,7 @@
       </c>
       <c r="E48" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>3.4437707009082885E-3</v>
+        <v>0.45763163339260127</v>
       </c>
       <c r="F48" s="1">
         <f t="shared" si="7"/>
@@ -5690,7 +5759,7 @@
       </c>
       <c r="E49" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.58997578322181621</v>
+        <v>1.7333636901204597E-2</v>
       </c>
       <c r="F49" s="1">
         <f t="shared" si="7"/>
@@ -5732,7 +5801,7 @@
       </c>
       <c r="E50" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.22900308435982564</v>
+        <v>0.53694166640104679</v>
       </c>
       <c r="F50" s="1">
         <f t="shared" si="7"/>
@@ -5774,7 +5843,7 @@
       </c>
       <c r="E51" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.26503365488684283</v>
+        <v>7.483525764513399E-2</v>
       </c>
       <c r="F51" s="1">
         <f t="shared" si="7"/>
@@ -5816,7 +5885,7 @@
       </c>
       <c r="E52" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89206696282837128</v>
+        <v>0.4424139348077476</v>
       </c>
       <c r="F52" s="1">
         <f t="shared" si="7"/>
@@ -5858,7 +5927,7 @@
       </c>
       <c r="E53" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.67426641438797541</v>
+        <v>0.59502538855494114</v>
       </c>
       <c r="F53" s="1">
         <f t="shared" si="7"/>
@@ -5900,7 +5969,7 @@
       </c>
       <c r="E54" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.45139253824195913</v>
+        <v>0.21856445610299291</v>
       </c>
       <c r="F54" s="1">
         <f t="shared" si="7"/>
@@ -5942,7 +6011,7 @@
       </c>
       <c r="E55" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.84995805546588865</v>
+        <v>0.8172571959224274</v>
       </c>
       <c r="F55" s="1">
         <f t="shared" si="7"/>
@@ -5984,7 +6053,7 @@
       </c>
       <c r="E56" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.29585987918101952</v>
+        <v>4.0708034557683126E-2</v>
       </c>
       <c r="F56" s="1">
         <f t="shared" si="7"/>
@@ -6026,7 +6095,7 @@
       </c>
       <c r="E57" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.39515285087034868</v>
+        <v>0.61068867259175519</v>
       </c>
       <c r="F57" s="1">
         <f t="shared" si="7"/>
@@ -6068,7 +6137,7 @@
       </c>
       <c r="E58" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85138736357872735</v>
+        <v>9.0067514363046053E-2</v>
       </c>
       <c r="F58" s="1">
         <f t="shared" si="7"/>
@@ -6110,7 +6179,7 @@
       </c>
       <c r="E59" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>3.5512090484848935E-2</v>
+        <v>0.22876533424402157</v>
       </c>
       <c r="F59" s="1">
         <f t="shared" si="7"/>
@@ -6152,7 +6221,7 @@
       </c>
       <c r="E60" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.19055117838157076</v>
+        <v>0.52414896315414816</v>
       </c>
       <c r="F60" s="1">
         <f t="shared" si="7"/>
@@ -6194,7 +6263,7 @@
       </c>
       <c r="E61" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4.6956325885031958E-2</v>
+        <v>0.53596351253127039</v>
       </c>
       <c r="F61" s="1">
         <f t="shared" si="7"/>
@@ -6236,7 +6305,7 @@
       </c>
       <c r="E62" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>5.2765765542790333E-2</v>
+        <v>0.82461804128641869</v>
       </c>
       <c r="F62" s="1">
         <f t="shared" si="7"/>
@@ -6278,7 +6347,7 @@
       </c>
       <c r="E63" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.26146311696499891</v>
+        <v>0.69117589719401118</v>
       </c>
       <c r="F63" s="1">
         <f t="shared" si="7"/>
@@ -6320,7 +6389,7 @@
       </c>
       <c r="E64" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.50935707946437658</v>
+        <v>0.6730558366401892</v>
       </c>
       <c r="F64" s="1">
         <f t="shared" si="7"/>
@@ -6362,7 +6431,7 @@
       </c>
       <c r="E65" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.82848704654883321</v>
+        <v>0.90606154506483616</v>
       </c>
       <c r="F65" s="1">
         <f t="shared" si="7"/>
@@ -6404,7 +6473,7 @@
       </c>
       <c r="E66" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.11122341122454049</v>
+        <v>3.4644253837764483E-2</v>
       </c>
       <c r="F66" s="1">
         <f t="shared" si="7"/>
@@ -6446,7 +6515,7 @@
       </c>
       <c r="E67" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.65785150323834862</v>
+        <v>9.935498821489086E-2</v>
       </c>
       <c r="F67" s="1">
         <f t="shared" si="7"/>
@@ -6468,7 +6537,7 @@
         <v>261</v>
       </c>
       <c r="M67" s="1" t="str">
-        <f t="shared" ref="M67:M114" si="11">",{""id"":""" &amp; C67 &amp; """,""date"":""" &amp; TEXT(B67, "mm/dd/yyyy") &amp; """,""word"":""" &amp; D67 &amp; """,""CLUE"":""" &amp; J67 &amp; """,""factoid"":""" &amp; K67 &amp; """,""url"":""" &amp; L67 &amp; """}"</f>
+        <f t="shared" ref="M67:M118" si="11">",{""id"":""" &amp; C67 &amp; """,""date"":""" &amp; TEXT(B67, "mm/dd/yyyy") &amp; """,""word"":""" &amp; D67 &amp; """,""CLUE"":""" &amp; J67 &amp; """,""factoid"":""" &amp; K67 &amp; """,""url"":""" &amp; L67 &amp; """}"</f>
         <v>,{"id":"23.5","date":"06/03/2022","word":"voodoo","CLUE":"","factoid":"(voo' doo) Some consider Voodoo a religion, some a form of witchcraft, and some just spooky fun. Whatever it is, it continues to fascinate visitors to New Orleans.","url":""}</v>
       </c>
     </row>
@@ -6488,7 +6557,7 @@
       </c>
       <c r="E68" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.90141872416780044</v>
+        <v>0.10596728054101912</v>
       </c>
       <c r="F68" s="1">
         <f t="shared" si="7"/>
@@ -6530,7 +6599,7 @@
       </c>
       <c r="E69" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8.292950594101689E-2</v>
+        <v>2.1460052612112146E-2</v>
       </c>
       <c r="F69" s="1">
         <f t="shared" si="7"/>
@@ -6572,7 +6641,7 @@
       </c>
       <c r="E70" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.96476164859954916</v>
+        <v>2.4951428410597831E-2</v>
       </c>
       <c r="F70" s="1">
         <f t="shared" si="7"/>
@@ -6614,7 +6683,7 @@
       </c>
       <c r="E71" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.76674922708345172</v>
+        <v>0.27548029061675661</v>
       </c>
       <c r="F71" s="1">
         <f t="shared" si="7"/>
@@ -6656,7 +6725,7 @@
       </c>
       <c r="E72" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.55417246216105631</v>
+        <v>2.906815355235115E-2</v>
       </c>
       <c r="F72" s="1">
         <f t="shared" si="7"/>
@@ -6698,7 +6767,7 @@
       </c>
       <c r="E73" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.4573036239933993</v>
+        <v>0.22294895578460949</v>
       </c>
       <c r="F73" s="1">
         <f t="shared" si="7"/>
@@ -6740,7 +6809,7 @@
       </c>
       <c r="E74" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.48184651589975735</v>
+        <v>0.44949663484744407</v>
       </c>
       <c r="F74" s="1">
         <f t="shared" si="7"/>
@@ -6782,7 +6851,7 @@
       </c>
       <c r="E75" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.44533571250498738</v>
+        <v>0.91807136291039548</v>
       </c>
       <c r="F75" s="1">
         <f t="shared" si="7"/>
@@ -6824,15 +6893,15 @@
       </c>
       <c r="E76" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.27210391102614928</v>
+        <v>0.30641631393003743</v>
       </c>
       <c r="F76" s="1">
-        <f t="shared" si="7"/>
-        <v>5</v>
+        <f>IF(ISNUMBER(SEARCH(" ",D110)), LEN(LEFT(D110,FIND(" ",D110)-1)), LEN(D110))</f>
+        <v>7</v>
       </c>
       <c r="G76" s="1">
-        <f t="shared" si="8"/>
-        <v>4</v>
+        <f>IF(ISNUMBER(SEARCH(" ",D110)), LEN(RIGHT(D110,LEN(D110)-FIND(" ",D110))), 0)</f>
+        <v>0</v>
       </c>
       <c r="H76" s="1" t="str">
         <f t="shared" si="9"/>
@@ -6840,19 +6909,19 @@
       </c>
       <c r="I76" s="1">
         <f t="shared" si="10"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K76" t="s">
         <v>277</v>
       </c>
       <c r="M76" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v>,{"id":"25.0","date":"06/12/2022","word":"front room","CLUE":"","factoid":"Known other places as the 'living room'.","url":""}</v>
+        <f>",{""id"":""" &amp; C76 &amp; """,""date"":""" &amp; TEXT(B76, "mm/dd/yyyy") &amp; """,""word"":""" &amp; D110 &amp; """,""CLUE"":""" &amp; J76 &amp; """,""factoid"":""" &amp; K76 &amp; """,""url"":""" &amp; L76 &amp; """}"</f>
+        <v>,{"id":"25.0","date":"06/12/2022","word":"tuition","CLUE":"","factoid":"Known other places as the 'living room'.","url":""}</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>93</v>
+        <v>310</v>
       </c>
       <c r="B77" s="2">
         <v>44725</v>
@@ -6862,18 +6931,18 @@
         <v>25.1</v>
       </c>
       <c r="D77" t="s">
-        <v>35</v>
+        <v>309</v>
       </c>
       <c r="E77" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.42872894604377987</v>
+        <v>0.82670976009409858</v>
       </c>
       <c r="F77" s="1">
-        <f t="shared" si="7"/>
+        <f>IF(ISNUMBER(SEARCH(" ",D111)), LEN(LEFT(D111,FIND(" ",D111)-1)), LEN(D111))</f>
         <v>5</v>
       </c>
       <c r="G77" s="1">
-        <f t="shared" si="8"/>
+        <f>IF(ISNUMBER(SEARCH(" ",D111)), LEN(RIGHT(D111,LEN(D111)-FIND(" ",D111))), 0)</f>
         <v>5</v>
       </c>
       <c r="H77" s="1" t="str">
@@ -6885,14 +6954,14 @@
         <v>10</v>
       </c>
       <c r="K77" t="s">
-        <v>133</v>
+        <v>311</v>
       </c>
       <c r="L77" s="8" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="M77" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v>,{"id":"25.1","date":"06/13/2022","word":"labor force","CLUE":"","factoid":"The labor force, as defined by the Bureau of Labor Statistics (BLS), is the number of people ages 16 and older who are either working or actively looking for work.","url":"https://www.shrm.org/resourcesandtools/tools-and-samples/hr-glossary/pages/labor-force.aspx"}</v>
+        <f>",{""id"":""" &amp; C77 &amp; """,""date"":""" &amp; TEXT(B77, "mm/dd/yyyy") &amp; """,""word"":""" &amp; D111 &amp; """,""CLUE"":""" &amp; J77 &amp; """,""factoid"":""" &amp; K77 &amp; """,""url"":""" &amp; L77 &amp; """}"</f>
+        <v>,{"id":"25.1","date":"06/13/2022","word":"labor force","CLUE":"","factoid":"63% of organizations said they offered some type of hybrid work opportunities in 2022. Additionally, 62% said they offer those employees with some type of subsidy or reimbursement for at home office or work equipment. Visit shrm.org/benefits to discover how your organization compares to others across flexible work and other types of benefits.","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
@@ -6911,14 +6980,14 @@
       </c>
       <c r="E78" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.81908149963885024</v>
+        <v>0.2399200092381768</v>
       </c>
       <c r="F78" s="1">
-        <f t="shared" si="7"/>
+        <f>IF(ISNUMBER(SEARCH(" ",D112)), LEN(LEFT(D112,FIND(" ",D112)-1)), LEN(D112))</f>
         <v>4</v>
       </c>
       <c r="G78" s="1">
-        <f t="shared" si="8"/>
+        <f>IF(ISNUMBER(SEARCH(" ",D112)), LEN(RIGHT(D112,LEN(D112)-FIND(" ",D112))), 0)</f>
         <v>6</v>
       </c>
       <c r="H78" s="1" t="str">
@@ -6936,13 +7005,13 @@
         <v>301</v>
       </c>
       <c r="M78" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f>",{""id"":""" &amp; C78 &amp; """,""date"":""" &amp; TEXT(B78, "mm/dd/yyyy") &amp; """,""word"":""" &amp; D112 &amp; """,""CLUE"":""" &amp; J78 &amp; """,""factoid"":""" &amp; K78 &amp; """,""url"":""" &amp; L78 &amp; """}"</f>
         <v>,{"id":"25.2","date":"06/14/2022","word":"soft skills","CLUE":"","factoid":"Soft skills are those related to behavioral and interpersonal abilities, such as the ability to effectively communicate, problem-solve, collaborate and organize. ","url":"https://www.shrm.org/resourcesandtools/tools-and-samples/hr-glossary/pages/soft-skills.aspx"}</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>94</v>
+        <v>310</v>
       </c>
       <c r="B79" s="2">
         <v>44727</v>
@@ -6952,18 +7021,18 @@
         <v>25.3</v>
       </c>
       <c r="D79" t="s">
-        <v>71</v>
+        <v>312</v>
       </c>
       <c r="E79" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85741545169592825</v>
+        <v>2.2286566982940514E-2</v>
       </c>
       <c r="F79" s="1">
-        <f t="shared" ref="F79:F91" si="13">IF(ISNUMBER(SEARCH(" ",D79)), LEN(LEFT(D79,FIND(" ",D79)-1)), LEN(D79))</f>
+        <f>IF(ISNUMBER(SEARCH(" ",D113)), LEN(LEFT(D113,FIND(" ",D113)-1)), LEN(D113))</f>
         <v>7</v>
       </c>
       <c r="G79" s="1">
-        <f t="shared" ref="G79:G91" si="14">IF(ISNUMBER(SEARCH(" ",D79)), LEN(RIGHT(D79,LEN(D79)-FIND(" ",D79))), 0)</f>
+        <f>IF(ISNUMBER(SEARCH(" ",D113)), LEN(RIGHT(D113,LEN(D113)-FIND(" ",D113))), 0)</f>
         <v>0</v>
       </c>
       <c r="H79" s="1" t="str">
@@ -6975,19 +7044,19 @@
         <v>7</v>
       </c>
       <c r="K79" t="s">
-        <v>190</v>
-      </c>
-      <c r="L79" t="s">
-        <v>187</v>
+        <v>313</v>
+      </c>
+      <c r="L79" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M79" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v>,{"id":"25.3","date":"06/15/2022","word":"account","CLUE":"","factoid":"Many employers offer different types of savings accounts to employees as benefits, such as flexible spending accounts or health savings accounts. Check out how many offer these savings plans in SHRM's Employee Benefits Survey. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <f>",{""id"":""" &amp; C79 &amp; """,""date"":""" &amp; TEXT(B79, "mm/dd/yyyy") &amp; """,""word"":""" &amp; D113 &amp; """,""CLUE"":""" &amp; J79 &amp; """,""factoid"":""" &amp; K79 &amp; """,""url"":""" &amp; L79 &amp; """}"</f>
+        <v>,{"id":"25.3","date":"06/15/2022","word":"account","CLUE":"","factoid":"In 2022, employers ranked retirement and savings benefits as among the most important types they can offer to employees. Most employers offered some type of retirement savings plan to their employees. Visit shrm.org/benefits to explore more retirement and savings benefits trends.","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>94</v>
+        <v>310</v>
       </c>
       <c r="B80" s="2">
         <v>44728</v>
@@ -7001,14 +7070,14 @@
       </c>
       <c r="E80" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.46677218808609433</v>
+        <v>0.81962446714877335</v>
       </c>
       <c r="F80" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="F79:F91" si="13">IF(ISNUMBER(SEARCH(" ",D80)), LEN(LEFT(D80,FIND(" ",D80)-1)), LEN(D80))</f>
         <v>6</v>
       </c>
       <c r="G80" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="G79:G91" si="14">IF(ISNUMBER(SEARCH(" ",D80)), LEN(RIGHT(D80,LEN(D80)-FIND(" ",D80))), 0)</f>
         <v>0</v>
       </c>
       <c r="H80" s="1" t="str">
@@ -7022,17 +7091,17 @@
       <c r="K80" t="s">
         <v>192</v>
       </c>
-      <c r="L80" t="s">
-        <v>187</v>
+      <c r="L80" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M80" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>,{"id":"25.4","date":"06/16/2022","word":"dental","CLUE":"","factoid":"98% of organizations offer dental insurance as an employee benefit in 2022. But there are many other benefits employees might offer to take care of their employees. Check out results from SHRM's Employee Benefits Survey to see how many of these benefits are offered by others. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"25.4","date":"06/16/2022","word":"dental","CLUE":"","factoid":"98% of organizations offer dental insurance as an employee benefit in 2022. But there are many other benefits employees might offer to take care of their employees. Check out results from SHRM's Employee Benefits Survey to see how many of these benefits are offered by others. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>94</v>
+        <v>310</v>
       </c>
       <c r="B81" s="2">
         <v>44729</v>
@@ -7046,7 +7115,7 @@
       </c>
       <c r="E81" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.70702595188951067</v>
+        <v>0.56326091337277162</v>
       </c>
       <c r="F81" s="1">
         <f t="shared" si="13"/>
@@ -7067,17 +7136,17 @@
       <c r="K81" t="s">
         <v>193</v>
       </c>
-      <c r="L81" t="s">
-        <v>187</v>
+      <c r="L81" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M81" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>,{"id":"25.5","date":"06/17/2022","word":"vision ","CLUE":"","factoid":"94% of organizations offer vision insurance as an employee benefit in 2022. But there are many other benefits employees might offer to take care of their employees. Check out results from SHRM's Employee Benefits Survey to see how many of these benefits are offered by others. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"25.5","date":"06/17/2022","word":"vision ","CLUE":"","factoid":"94% of organizations offer vision insurance as an employee benefit in 2022. But there are many other benefits employees might offer to take care of their employees. Check out results from SHRM's Employee Benefits Survey to see how many of these benefits are offered by others. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>94</v>
+        <v>310</v>
       </c>
       <c r="B82" s="2">
         <v>44730</v>
@@ -7091,7 +7160,7 @@
       </c>
       <c r="E82" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.55230225680344536</v>
+        <v>0.20026132926480766</v>
       </c>
       <c r="F82" s="1">
         <f t="shared" si="13"/>
@@ -7112,17 +7181,17 @@
       <c r="K82" t="s">
         <v>194</v>
       </c>
-      <c r="L82" t="s">
-        <v>187</v>
+      <c r="L82" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M82" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>,{"id":"25.6","date":"06/18/2022","word":"health","CLUE":"","factoid":"Benefits focusing on employee health are a great tool employers can use to attract the best talent but more importantly, to keep their employees safe. Check out SHRM's Employee Benefits Survey to see which health-related benefits were among those most often offered. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"25.6","date":"06/18/2022","word":"health","CLUE":"","factoid":"Benefits focusing on employee health are a great tool employers can use to attract the best talent but more importantly, to keep their employees safe. Check out SHRM's Employee Benefits Survey to see which health-related benefits were among those most often offered. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>94</v>
+        <v>310</v>
       </c>
       <c r="B83" s="2">
         <v>44731</v>
@@ -7136,7 +7205,7 @@
       </c>
       <c r="E83" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.11549409834314361</v>
+        <v>0.62749842062403471</v>
       </c>
       <c r="F83" s="1">
         <f t="shared" si="13"/>
@@ -7157,17 +7226,17 @@
       <c r="K83" t="s">
         <v>195</v>
       </c>
-      <c r="L83" t="s">
-        <v>187</v>
+      <c r="L83" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M83" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>,{"id":"26.0","date":"06/19/2022","word":"mental","CLUE":"","factoid":"More employers than ever offered employees mental health benefits in 2022 than ever before. See what other health and wellness benefits were offered in SHRM's Employee Benefits Survey. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"26.0","date":"06/19/2022","word":"mental","CLUE":"","factoid":"More employers than ever offered employees mental health benefits in 2022 than ever before. See what other health and wellness benefits were offered in SHRM's Employee Benefits Survey. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>94</v>
+        <v>310</v>
       </c>
       <c r="B84" s="2">
         <v>44732</v>
@@ -7181,7 +7250,7 @@
       </c>
       <c r="E84" s="1">
         <f t="shared" ref="E84:E118" ca="1" si="15">RAND()</f>
-        <v>0.31979384869598582</v>
+        <v>0.67124429289580967</v>
       </c>
       <c r="F84" s="1">
         <f t="shared" si="13"/>
@@ -7202,17 +7271,17 @@
       <c r="K84" t="s">
         <v>196</v>
       </c>
-      <c r="L84" t="s">
-        <v>187</v>
+      <c r="L84" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M84" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>,{"id":"26.1","date":"06/20/2022","word":"rewards","CLUE":"","factoid":"Offering employees rewards for participating in health and wellness programs is a great benefits you can offer to encourage employees to take care of themselves. See what other health and wellness beneifts were offered in SHRM's Employee Benefits Survey. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"26.1","date":"06/20/2022","word":"rewards","CLUE":"","factoid":"Offering employees rewards for participating in health and wellness programs is a great benefits you can offer to encourage employees to take care of themselves. See what other health and wellness beneifts were offered in SHRM's Employee Benefits Survey. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>94</v>
+        <v>310</v>
       </c>
       <c r="B85" s="2">
         <v>44733</v>
@@ -7226,7 +7295,7 @@
       </c>
       <c r="E85" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.85363167557001207</v>
+        <v>0.61758216071040362</v>
       </c>
       <c r="F85" s="1">
         <f t="shared" si="13"/>
@@ -7247,17 +7316,17 @@
       <c r="K85" t="s">
         <v>198</v>
       </c>
-      <c r="L85" t="s">
-        <v>187</v>
+      <c r="L85" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M85" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>,{"id":"26.2","date":"06/21/2022","word":"coach","CLUE":"","factoid":"Employers can provide access to various types of coaches or specialists as a benefit, such as nutritional or life coaching. Check out results from SHRM's Employee Benefits Survey to learn what types of benefits organizations are offering. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"26.2","date":"06/21/2022","word":"coach","CLUE":"","factoid":"Employers can provide access to various types of coaches or specialists as a benefit, such as nutritional or life coaching. Check out results from SHRM's Employee Benefits Survey to learn what types of benefits organizations are offering. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>94</v>
+        <v>310</v>
       </c>
       <c r="B86" s="2">
         <v>44734</v>
@@ -7271,7 +7340,7 @@
       </c>
       <c r="E86" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.46580845226362189</v>
+        <v>0.89584207684299522</v>
       </c>
       <c r="F86" s="1">
         <f t="shared" si="13"/>
@@ -7292,12 +7361,12 @@
       <c r="K86" t="s">
         <v>199</v>
       </c>
-      <c r="L86" t="s">
-        <v>187</v>
+      <c r="L86" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M86" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>,{"id":"26.3","date":"06/22/2022","word":"leave","CLUE":"","factoid":"Leave continues to be ranked among the most important types of benefits employers believe they can offer. Learn more about the types of leave and other benefits in SHRM's Employee Benefits Survey. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"26.3","date":"06/22/2022","word":"leave","CLUE":"","factoid":"Leave continues to be ranked among the most important types of benefits employers believe they can offer. Learn more about the types of leave and other benefits in SHRM's Employee Benefits Survey. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
@@ -7316,7 +7385,7 @@
       </c>
       <c r="E87" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.61742468241377502</v>
+        <v>0.23226561309029181</v>
       </c>
       <c r="F87" s="1">
         <f t="shared" si="13"/>
@@ -7347,7 +7416,7 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>94</v>
+        <v>310</v>
       </c>
       <c r="B88" s="2">
         <v>44736</v>
@@ -7361,7 +7430,7 @@
       </c>
       <c r="E88" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.62654493119586008</v>
+        <v>0.52130762452210033</v>
       </c>
       <c r="F88" s="1">
         <f t="shared" si="13"/>
@@ -7382,17 +7451,17 @@
       <c r="K88" t="s">
         <v>211</v>
       </c>
-      <c r="L88" t="s">
-        <v>187</v>
+      <c r="L88" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M88" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>,{"id":"26.5","date":"06/24/2022","word":"mentor","CLUE":"","factoid":"Mentorship programs are a great way in which employers can allow employees to connect and learn from each other. Find out how many organizations offered a mentorship program by visiting SHRM's Employee Benefits Survey. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"26.5","date":"06/24/2022","word":"mentor","CLUE":"","factoid":"Mentorship programs are a great way in which employers can allow employees to connect and learn from each other. Find out how many organizations offered a mentorship program by visiting SHRM's Employee Benefits Survey. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>94</v>
+        <v>310</v>
       </c>
       <c r="B89" s="2">
         <v>44737</v>
@@ -7406,7 +7475,7 @@
       </c>
       <c r="E89" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.49024558660659368</v>
+        <v>0.12743136631549778</v>
       </c>
       <c r="F89" s="1">
         <f t="shared" si="13"/>
@@ -7427,17 +7496,17 @@
       <c r="K89" t="s">
         <v>210</v>
       </c>
-      <c r="L89" t="s">
-        <v>187</v>
+      <c r="L89" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M89" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>,{"id":"26.6","date":"06/25/2022","word":"paycard","CLUE":"","factoid":"Paycards allow employers to provide employees with compensation by transfering funds to a debit card rather than to an employee's bank account. Find out how many offered this and other types of benefits by visiting SHRM's Employee Benefits Survey. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"26.6","date":"06/25/2022","word":"paycard","CLUE":"","factoid":"Paycards allow employers to provide employees with compensation by transfering funds to a debit card rather than to an employee's bank account. Find out how many offered this and other types of benefits by visiting SHRM's Employee Benefits Survey. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>94</v>
+        <v>310</v>
       </c>
       <c r="B90" s="2">
         <v>44738</v>
@@ -7451,7 +7520,7 @@
       </c>
       <c r="E90" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.78441420499708114</v>
+        <v>0.6000038806849689</v>
       </c>
       <c r="F90" s="1">
         <f t="shared" si="13"/>
@@ -7472,17 +7541,17 @@
       <c r="K90" t="s">
         <v>188</v>
       </c>
-      <c r="L90" t="s">
-        <v>187</v>
+      <c r="L90" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M90" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>,{"id":"27.0","date":"06/26/2022","word":"benefit","CLUE":"","factoid":"Non-wage forms of compensation offered to employees in exchange for work. While many organizations offer many of the same types of benefits, there are almost always differences between them. Check out SHRM's Employee Benefit Survey to see how many organizations offer different types of benefits. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"27.0","date":"06/26/2022","word":"benefit","CLUE":"","factoid":"Non-wage forms of compensation offered to employees in exchange for work. While many organizations offer many of the same types of benefits, there are almost always differences between them. Check out SHRM's Employee Benefit Survey to see how many organizations offer different types of benefits. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>94</v>
+        <v>310</v>
       </c>
       <c r="B91" s="2">
         <v>44739</v>
@@ -7496,7 +7565,7 @@
       </c>
       <c r="E91" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>2.8445989005350336E-2</v>
+        <v>0.96071331746400657</v>
       </c>
       <c r="F91" s="1">
         <f t="shared" si="13"/>
@@ -7517,17 +7586,17 @@
       <c r="K91" t="s">
         <v>189</v>
       </c>
-      <c r="L91" t="s">
-        <v>187</v>
+      <c r="L91" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M91" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>,{"id":"27.1","date":"06/27/2022","word":"hdhp","CLUE":"","factoid":"High-deductible health plans (HDHPs) are health insurance plans an organization may offer. Typically, these plans are either linked with health savings plans or not. Check out how many organizations offer HDHPs in SHRM's Employee Benefits Survey. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"27.1","date":"06/27/2022","word":"hdhp","CLUE":"","factoid":"High-deductible health plans (HDHPs) are health insurance plans an organization may offer. Typically, these plans are either linked with health savings plans or not. Check out how many organizations offer HDHPs in SHRM's Employee Benefits Survey. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>94</v>
+        <v>310</v>
       </c>
       <c r="B92" s="2">
         <v>44740</v>
@@ -7541,7 +7610,7 @@
       </c>
       <c r="E92" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.1980021571810433</v>
+        <v>0.73531113815225202</v>
       </c>
       <c r="F92" s="1">
         <f t="shared" ref="F92:F106" si="16">IF(ISNUMBER(SEARCH(" ",D92)), LEN(LEFT(D92,FIND(" ",D92)-1)), LEN(D92))</f>
@@ -7562,17 +7631,17 @@
       <c r="K92" t="s">
         <v>204</v>
       </c>
-      <c r="L92" t="s">
-        <v>187</v>
+      <c r="L92" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M92" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>,{"id":"27.2","date":"06/28/2022","word":"federal","CLUE":"","factoid":"Federal law requires certain organizations to offer employees with a minimum amount of unpaid leave to care for their families. Some organizations offer more than the minimum, however. Find out how many by visiting SHRM's Employee Benefits Survey. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"27.2","date":"06/28/2022","word":"federal","CLUE":"","factoid":"Federal law requires certain organizations to offer employees with a minimum amount of unpaid leave to care for their families. Some organizations offer more than the minimum, however. Find out how many by visiting SHRM's Employee Benefits Survey. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>94</v>
+        <v>310</v>
       </c>
       <c r="B93" s="2">
         <v>44741</v>
@@ -7586,7 +7655,7 @@
       </c>
       <c r="E93" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.77679971216576627</v>
+        <v>0.19394999645210365</v>
       </c>
       <c r="F93" s="1">
         <f t="shared" si="16"/>
@@ -7607,17 +7676,17 @@
       <c r="K93" t="s">
         <v>205</v>
       </c>
-      <c r="L93" t="s">
-        <v>187</v>
+      <c r="L93" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M93" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>,{"id":"27.3","date":"06/29/2022","word":"roth","CLUE":"","factoid":"A Roth 401(k) or similar retirement plans have slowly been increasing in prevalence over the past five years. Find out how many organizations offer these and other retirement plans in SHRM's Employee Benefits Survey. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"27.3","date":"06/29/2022","word":"roth","CLUE":"","factoid":"A Roth 401(k) or similar retirement plans have slowly been increasing in prevalence over the past five years. Find out how many organizations offer these and other retirement plans in SHRM's Employee Benefits Survey. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>94</v>
+        <v>310</v>
       </c>
       <c r="B94" s="2">
         <v>44742</v>
@@ -7631,7 +7700,7 @@
       </c>
       <c r="E94" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.61706648874670966</v>
+        <v>7.7692247055833219E-2</v>
       </c>
       <c r="F94" s="1">
         <f t="shared" si="16"/>
@@ -7652,17 +7721,17 @@
       <c r="K94" t="s">
         <v>206</v>
       </c>
-      <c r="L94" t="s">
-        <v>187</v>
+      <c r="L94" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M94" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>,{"id":"27.4","date":"06/30/2022","word":"match","CLUE":"","factoid":"Employers can offer retirement plan and health savings matches as an employee benefit. Find out how many do by visiting SHRM's Employee Benefits Survey. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"27.4","date":"06/30/2022","word":"match","CLUE":"","factoid":"Employers can offer retirement plan and health savings matches as an employee benefit. Find out how many do by visiting SHRM's Employee Benefits Survey. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>94</v>
+        <v>310</v>
       </c>
       <c r="B95" s="2">
         <v>44743</v>
@@ -7676,7 +7745,7 @@
       </c>
       <c r="E95" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.98280137410062485</v>
+        <v>0.1398123386377027</v>
       </c>
       <c r="F95" s="1">
         <f t="shared" si="16"/>
@@ -7697,17 +7766,17 @@
       <c r="K95" t="s">
         <v>207</v>
       </c>
-      <c r="L95" t="s">
-        <v>187</v>
+      <c r="L95" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M95" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>,{"id":"27.5","date":"07/01/2022","word":"child","CLUE":"","factoid":"Employers can offer benefits related to child care as an employee benefit - a great way to help out those employees who are also working parents. Find out how many offer these benefits by visiting SHRM's Benefits Survey. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"27.5","date":"07/01/2022","word":"child","CLUE":"","factoid":"Employers can offer benefits related to child care as an employee benefit - a great way to help out those employees who are also working parents. Find out how many offer these benefits by visiting SHRM's Benefits Survey. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>94</v>
+        <v>310</v>
       </c>
       <c r="B96" s="2">
         <v>44744</v>
@@ -7721,7 +7790,7 @@
       </c>
       <c r="E96" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.28332830448333735</v>
+        <v>0.99061452826238361</v>
       </c>
       <c r="F96" s="1">
         <f t="shared" si="16"/>
@@ -7742,17 +7811,17 @@
       <c r="K96" t="s">
         <v>208</v>
       </c>
-      <c r="L96" t="s">
-        <v>187</v>
+      <c r="L96" s="8" t="s">
+        <v>308</v>
       </c>
       <c r="M96" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>,{"id":"27.6","date":"07/02/2022","word":"elder","CLUE":"","factoid":"Aging populations leave many workers responsible with worrying about elder care. Employers can offer resources to help. Find out how many offer these and other types of benefits in SHRM's Employee Benefits Survey. ","url":"https://www.shrm.org/hr-today/trends-and-forecasting/research-and-surveys/pages/benefits-report.aspx"}</v>
+        <v>,{"id":"27.6","date":"07/02/2022","word":"elder","CLUE":"","factoid":"Aging populations leave many workers responsible with worrying about elder care. Employers can offer resources to help. Find out how many offer these and other types of benefits in SHRM's Employee Benefits Survey. ","url":"https://shrm.org/benefits"}</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>94</v>
+        <v>310</v>
       </c>
       <c r="B97" s="2">
         <v>44745</v>
@@ -7766,7 +7835,7 @@
       </c>
       <c r="E97" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>7.8672425559948356E-2</v>
+        <v>0.74511317116830023</v>
       </c>
       <c r="F97" s="1">
         <f t="shared" si="16"/>
@@ -7787,7 +7856,7 @@
       <c r="K97" t="s">
         <v>209</v>
       </c>
-      <c r="L97" t="s">
+      <c r="L97" s="8" t="s">
         <v>187</v>
       </c>
       <c r="M97" s="1" t="str">
@@ -7811,7 +7880,7 @@
       </c>
       <c r="E98" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.1995195548947224</v>
+        <v>0.69970713786151351</v>
       </c>
       <c r="F98" s="1">
         <f t="shared" si="16"/>
@@ -7856,7 +7925,7 @@
       </c>
       <c r="E99" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.31655503526899642</v>
+        <v>0.76321688821145528</v>
       </c>
       <c r="F99" s="1">
         <f t="shared" si="16"/>
@@ -7901,7 +7970,7 @@
       </c>
       <c r="E100" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.74419921129782407</v>
+        <v>0.80185765557612176</v>
       </c>
       <c r="F100" s="1">
         <f t="shared" si="16"/>
@@ -7946,7 +8015,7 @@
       </c>
       <c r="E101" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.16739494412430267</v>
+        <v>0.86949061700481933</v>
       </c>
       <c r="F101" s="1">
         <f t="shared" si="16"/>
@@ -7991,7 +8060,7 @@
       </c>
       <c r="E102" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.74959000573067303</v>
+        <v>0.7527943431278169</v>
       </c>
       <c r="F102" s="1">
         <f t="shared" si="16"/>
@@ -8036,7 +8105,7 @@
       </c>
       <c r="E103" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>1.3253554960209413E-2</v>
+        <v>0.88544934027608746</v>
       </c>
       <c r="F103" s="1">
         <f t="shared" si="16"/>
@@ -8081,7 +8150,7 @@
       </c>
       <c r="E104" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.36823440157987652</v>
+        <v>0.62366702219930159</v>
       </c>
       <c r="F104" s="1">
         <f t="shared" si="16"/>
@@ -8126,7 +8195,7 @@
       </c>
       <c r="E105" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.43185908785361016</v>
+        <v>0.2356513213320125</v>
       </c>
       <c r="F105" s="1">
         <f t="shared" si="16"/>
@@ -8171,7 +8240,7 @@
       </c>
       <c r="E106" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.24650641742811086</v>
+        <v>1.2398733737589485E-2</v>
       </c>
       <c r="F106" s="1">
         <f t="shared" si="16"/>
@@ -8216,10 +8285,10 @@
       </c>
       <c r="E107" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.58231521893274685</v>
+        <v>0.46601224536422325</v>
       </c>
       <c r="F107" s="1">
-        <f t="shared" ref="F107:F114" si="20">IF(ISNUMBER(SEARCH(" ",D107)), LEN(LEFT(D107,FIND(" ",D107)-1)), LEN(D107))</f>
+        <f t="shared" ref="F107:F118" si="20">IF(ISNUMBER(SEARCH(" ",D107)), LEN(LEFT(D107,FIND(" ",D107)-1)), LEN(D107))</f>
         <v>3</v>
       </c>
       <c r="G107" s="1">
@@ -8261,7 +8330,7 @@
       </c>
       <c r="E108" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.28340174787194894</v>
+        <v>0.92073887484308536</v>
       </c>
       <c r="F108" s="1">
         <f t="shared" si="20"/>
@@ -8306,7 +8375,7 @@
       </c>
       <c r="E109" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.61152070850163598</v>
+        <v>0.79322847536804197</v>
       </c>
       <c r="F109" s="1">
         <f t="shared" si="20"/>
@@ -8337,7 +8406,7 @@
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>93</v>
+        <v>310</v>
       </c>
       <c r="B110" s="2">
         <v>44758</v>
@@ -8346,16 +8415,19 @@
         <f t="shared" si="19"/>
         <v>29.6</v>
       </c>
+      <c r="D110" t="s">
+        <v>314</v>
+      </c>
       <c r="E110" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.17803279392727678</v>
+        <v>0.23204017130718813</v>
       </c>
       <c r="F110" s="1">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G110" s="1">
-        <f t="shared" si="21"/>
+        <f>IF(ISNUMBER(SEARCH(" ",#REF!)), LEN(RIGHT(#REF!,LEN(#REF!)-FIND(" ",#REF!))), 0)</f>
         <v>0</v>
       </c>
       <c r="H110" s="1" t="str">
@@ -8364,9 +8436,18 @@
       </c>
       <c r="I110" s="1">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="M110" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="K110" t="s">
+        <v>315</v>
+      </c>
+      <c r="L110" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="M110" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>,{"id":"29.6","date":"07/16/2022","word":"tuition","CLUE":"","factoid":"Nearly half of organizations (48%) offer undergraduate or graduate tuition assistance as an employee benefit. There are many other ways in which organizations use benefits to support their employees’ professional development and growth. Visit shrm.org/benefits to discover how your organization compares to others across these and other types of benefits.","url":"https://shrm.org/benefits"}</v>
+      </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
@@ -8379,16 +8460,19 @@
         <f t="shared" si="19"/>
         <v>30.0</v>
       </c>
+      <c r="D111" t="s">
+        <v>35</v>
+      </c>
       <c r="E111" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.96626756781972678</v>
+        <v>0.7852802472387137</v>
       </c>
       <c r="F111" s="1">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G111" s="1">
-        <f t="shared" si="21"/>
+        <f>IF(ISNUMBER(SEARCH(" ",#REF!)), LEN(RIGHT(#REF!,LEN(#REF!)-FIND(" ",#REF!))), 0)</f>
         <v>0</v>
       </c>
       <c r="H111" s="1" t="str">
@@ -8397,9 +8481,18 @@
       </c>
       <c r="I111" s="1">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="M111" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="K111" t="s">
+        <v>133</v>
+      </c>
+      <c r="L111" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="M111" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>,{"id":"30.0","date":"07/17/2022","word":"labor force","CLUE":"","factoid":"The labor force, as defined by the Bureau of Labor Statistics (BLS), is the number of people ages 16 and older who are either working or actively looking for work.","url":"https://www.shrm.org/resourcesandtools/tools-and-samples/hr-glossary/pages/labor-force.aspx"}</v>
+      </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
@@ -8412,16 +8505,19 @@
         <f t="shared" si="19"/>
         <v>30.1</v>
       </c>
+      <c r="D112" t="s">
+        <v>37</v>
+      </c>
       <c r="E112" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.93396476202421186</v>
+        <v>0.24148774768879211</v>
       </c>
       <c r="F112" s="1">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G112" s="1">
-        <f t="shared" si="21"/>
+        <f>IF(ISNUMBER(SEARCH(" ",#REF!)), LEN(RIGHT(#REF!,LEN(#REF!)-FIND(" ",#REF!))), 0)</f>
         <v>0</v>
       </c>
       <c r="H112" s="1" t="str">
@@ -8430,15 +8526,22 @@
       </c>
       <c r="I112" s="1">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K112" s="3"/>
-      <c r="L112" s="3"/>
-      <c r="M112" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="K112" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="L112" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="M112" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>,{"id":"30.1","date":"07/18/2022","word":"soft skills","CLUE":"","factoid":"Soft skills are those related to behavioral and interpersonal abilities, such as the ability to effectively communicate, problem-solve, collaborate and organize. ","url":"https://www.shrm.org/resourcesandtools/tools-and-samples/hr-glossary/pages/soft-skills.aspx"}</v>
+      </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>93</v>
+        <v>310</v>
       </c>
       <c r="B113" s="2">
         <v>44761</v>
@@ -8447,16 +8550,19 @@
         <f t="shared" si="19"/>
         <v>30.2</v>
       </c>
+      <c r="D113" t="s">
+        <v>71</v>
+      </c>
       <c r="E113" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.38655669279222293</v>
+        <v>0.2495473579289641</v>
       </c>
       <c r="F113" s="1">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G113" s="1">
-        <f t="shared" si="21"/>
+        <f>IF(ISNUMBER(SEARCH(" ",#REF!)), LEN(RIGHT(#REF!,LEN(#REF!)-FIND(" ",#REF!))), 0)</f>
         <v>0</v>
       </c>
       <c r="H113" s="1" t="str">
@@ -8465,15 +8571,22 @@
       </c>
       <c r="I113" s="1">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K113" s="3"/>
-      <c r="L113" s="8"/>
-      <c r="M113" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="K113" t="s">
+        <v>190</v>
+      </c>
+      <c r="L113" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="M113" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>,{"id":"30.2","date":"07/19/2022","word":"account","CLUE":"","factoid":"Many employers offer different types of savings accounts to employees as benefits, such as flexible spending accounts or health savings accounts. Check out how many offer these savings plans in SHRM's Employee Benefits Survey. ","url":"https://shrm.org/benefits"}</v>
+      </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>93</v>
+        <v>310</v>
       </c>
       <c r="B114" s="2">
         <v>44762</v>
@@ -8482,13 +8595,16 @@
         <f t="shared" si="19"/>
         <v>30.3</v>
       </c>
+      <c r="D114" t="s">
+        <v>316</v>
+      </c>
       <c r="E114" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.67662125966221687</v>
+        <v>0.73873463368512871</v>
       </c>
       <c r="F114" s="1">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G114" s="1">
         <f t="shared" si="21"/>
@@ -8500,10 +8616,18 @@
       </c>
       <c r="I114" s="1">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="L114" s="8"/>
-      <c r="M114" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="K114" t="s">
+        <v>317</v>
+      </c>
+      <c r="L114" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="M114" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>,{"id":"30.3","date":"07/20/2022","word":"program","CLUE":"","factoid":"Employers can offer several types of programs that focus of health and wellbeing as an employee benefit. These programs can include weight loss, tobacco cessation, and general wellness programs covering many health-related areas. Visit shrm.org/benefits to discover how your organization compares to others across these and other types of benefits.","url":"https://shrm.org/benefits"}</v>
+      </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
@@ -8518,10 +8642,10 @@
       </c>
       <c r="E115" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.47412253676326388</v>
+        <v>0.67565993554617287</v>
       </c>
       <c r="F115" s="1">
-        <f>IF(ISNUMBER(SEARCH(" ",D115)), LEN(LEFT(D115,FIND(" ",D115)-1)), LEN(D115))</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="G115" s="1">
@@ -8552,10 +8676,10 @@
       </c>
       <c r="E116" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.53283080416388517</v>
+        <v>0.7771445924210344</v>
       </c>
       <c r="F116" s="1">
-        <f>IF(ISNUMBER(SEARCH(" ",D116)), LEN(LEFT(D116,FIND(" ",D116)-1)), LEN(D116))</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="G116" s="1">
@@ -8586,14 +8710,14 @@
       </c>
       <c r="E117" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.29094888541615849</v>
+        <v>0.49656939524760424</v>
       </c>
       <c r="F117" s="1">
-        <f t="shared" ref="F117:F118" si="23">IF(ISNUMBER(SEARCH(" ",D117)), LEN(LEFT(D117,FIND(" ",D117)-1)), LEN(D117))</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="G117" s="1">
-        <f t="shared" ref="G117:G118" si="24">IF(ISNUMBER(SEARCH(" ",D117)), LEN(RIGHT(D117,LEN(D117)-FIND(" ",D117))), 0)</f>
+        <f t="shared" ref="G117:G118" si="23">IF(ISNUMBER(SEARCH(" ",D117)), LEN(RIGHT(D117,LEN(D117)-FIND(" ",D117))), 0)</f>
         <v>0</v>
       </c>
       <c r="H117" s="1" t="str">
@@ -8604,6 +8728,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
+      <c r="M117" s="1"/>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
@@ -8618,14 +8743,14 @@
       </c>
       <c r="E118" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>0.46055227963227097</v>
+        <v>0.44251929704134429</v>
       </c>
       <c r="F118" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="G118" s="1">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="G118" s="1">
-        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="H118" s="1" t="str">
@@ -8636,211 +8761,230 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
+      <c r="M118" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M118" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="H2:H1048576">
-    <cfRule type="containsText" dxfId="132" priority="35" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="135" priority="38" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="107">
+    <cfRule type="containsBlanks" priority="110">
       <formula>LEN(TRIM(H2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048576">
-    <cfRule type="cellIs" dxfId="131" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="134" priority="39" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K30 K119:K1048576 K79:K88 K90:K101 K45:K77">
-    <cfRule type="containsText" dxfId="130" priority="119" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="133" priority="122" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G1048576">
-    <cfRule type="cellIs" dxfId="129" priority="45" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="132" priority="48" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsBlanks" dxfId="128" priority="34">
+  <conditionalFormatting sqref="D1:D75 D77 D79:D1048576">
+    <cfRule type="containsBlanks" dxfId="131" priority="37">
       <formula>LEN(TRIM(D1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K99:K103 K110:K112">
+  <conditionalFormatting sqref="K99:K103 K110">
+    <cfRule type="containsText" dxfId="130" priority="36" operator="containsText" text="&quot;">
+      <formula>NOT(ISERROR(SEARCH("""",K99)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K116">
+    <cfRule type="containsText" dxfId="129" priority="35" operator="containsText" text="&quot;">
+      <formula>NOT(ISERROR(SEARCH("""",K116)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K117">
+    <cfRule type="containsText" dxfId="128" priority="34" operator="containsText" text="&quot;">
+      <formula>NOT(ISERROR(SEARCH("""",K117)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K118">
     <cfRule type="containsText" dxfId="127" priority="33" operator="containsText" text="&quot;">
-      <formula>NOT(ISERROR(SEARCH("""",K99)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K116">
+      <formula>NOT(ISERROR(SEARCH("""",K118)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K90">
     <cfRule type="containsText" dxfId="126" priority="32" operator="containsText" text="&quot;">
-      <formula>NOT(ISERROR(SEARCH("""",K116)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K117">
+      <formula>NOT(ISERROR(SEARCH("""",K90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K91">
     <cfRule type="containsText" dxfId="125" priority="31" operator="containsText" text="&quot;">
-      <formula>NOT(ISERROR(SEARCH("""",K117)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K118">
+      <formula>NOT(ISERROR(SEARCH("""",K91)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K89">
     <cfRule type="containsText" dxfId="124" priority="30" operator="containsText" text="&quot;">
-      <formula>NOT(ISERROR(SEARCH("""",K118)))</formula>
+      <formula>NOT(ISERROR(SEARCH("""",K89)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K115">
+    <cfRule type="containsText" dxfId="123" priority="29" operator="containsText" text="&quot;">
+      <formula>NOT(ISERROR(SEARCH("""",K115)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K89">
+    <cfRule type="containsText" dxfId="122" priority="28" operator="containsText" text="&quot;">
+      <formula>NOT(ISERROR(SEARCH("""",K89)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K90">
-    <cfRule type="containsText" dxfId="123" priority="29" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="121" priority="27" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K90)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K91">
-    <cfRule type="containsText" dxfId="122" priority="28" operator="containsText" text="&quot;">
-      <formula>NOT(ISERROR(SEARCH("""",K91)))</formula>
+  <conditionalFormatting sqref="K88">
+    <cfRule type="containsText" dxfId="120" priority="26" operator="containsText" text="&quot;">
+      <formula>NOT(ISERROR(SEARCH("""",K88)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K114">
+    <cfRule type="containsText" dxfId="119" priority="25" operator="containsText" text="&quot;">
+      <formula>NOT(ISERROR(SEARCH("""",K114)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K89">
-    <cfRule type="containsText" dxfId="121" priority="27" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="118" priority="24" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K89)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K115">
-    <cfRule type="containsText" dxfId="120" priority="26" operator="containsText" text="&quot;">
-      <formula>NOT(ISERROR(SEARCH("""",K115)))</formula>
+  <conditionalFormatting sqref="K90">
+    <cfRule type="containsText" dxfId="117" priority="23" operator="containsText" text="&quot;">
+      <formula>NOT(ISERROR(SEARCH("""",K90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K88">
+    <cfRule type="containsText" dxfId="116" priority="22" operator="containsText" text="&quot;">
+      <formula>NOT(ISERROR(SEARCH("""",K88)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K88">
+    <cfRule type="containsText" dxfId="115" priority="21" operator="containsText" text="&quot;">
+      <formula>NOT(ISERROR(SEARCH("""",K88)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K89">
-    <cfRule type="containsText" dxfId="119" priority="25" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="114" priority="20" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K89)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K90">
-    <cfRule type="containsText" dxfId="118" priority="24" operator="containsText" text="&quot;">
-      <formula>NOT(ISERROR(SEARCH("""",K90)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K88">
-    <cfRule type="containsText" dxfId="117" priority="23" operator="containsText" text="&quot;">
-      <formula>NOT(ISERROR(SEARCH("""",K88)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K114">
-    <cfRule type="containsText" dxfId="116" priority="22" operator="containsText" text="&quot;">
-      <formula>NOT(ISERROR(SEARCH("""",K114)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K89">
-    <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="&quot;">
-      <formula>NOT(ISERROR(SEARCH("""",K89)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K90">
-    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="&quot;">
-      <formula>NOT(ISERROR(SEARCH("""",K90)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K88">
-    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="&quot;">
-      <formula>NOT(ISERROR(SEARCH("""",K88)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K88">
-    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="&quot;">
-      <formula>NOT(ISERROR(SEARCH("""",K88)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K89">
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="&quot;">
-      <formula>NOT(ISERROR(SEARCH("""",K89)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K87">
-    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="113" priority="19" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K104">
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="112" priority="18" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K104)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K105:K107">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="111" priority="17" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K105)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K109">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="110" priority="16" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K109)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31 K33:K42 K44">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="109" priority="15" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="108" priority="14" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K43">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="107" priority="13" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K43">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="106" priority="12" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="105" priority="11" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="104" priority="10" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K43">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="103" priority="9" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="102" priority="8" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="101" priority="7" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42">
+    <cfRule type="containsText" dxfId="100" priority="6" operator="containsText" text="&quot;">
+      <formula>NOT(ISERROR(SEARCH("""",K42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K43">
+    <cfRule type="containsText" dxfId="99" priority="5" operator="containsText" text="&quot;">
+      <formula>NOT(ISERROR(SEARCH("""",K43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K41">
+    <cfRule type="containsText" dxfId="98" priority="4" operator="containsText" text="&quot;">
+      <formula>NOT(ISERROR(SEARCH("""",K41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K113 K111">
     <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="&quot;">
-      <formula>NOT(ISERROR(SEARCH("""",K42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K43">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="&quot;">
-      <formula>NOT(ISERROR(SEARCH("""",K43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K41">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="&quot;">
-      <formula>NOT(ISERROR(SEARCH("""",K41)))</formula>
+      <formula>NOT(ISERROR(SEARCH("""",K111)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D76">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(D76))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D78">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(D78))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="L78" r:id="rId1" xr:uid="{C68E4A8B-CDD2-C849-A41A-91099F8BB181}"/>
-    <hyperlink ref="L77" r:id="rId2" xr:uid="{99A89A2F-EDE1-784D-9C13-89314428F069}"/>
-    <hyperlink ref="L108" r:id="rId3" display="https://www.shrm.org/resourcesandtools/tools-and-samples/hr-glossary/pages/soft-skills.aspx" xr:uid="{11470350-D5B9-3F44-99ED-2B7C2330DD6C}"/>
-    <hyperlink ref="L109" r:id="rId4" display="https://www.shrm.org/resourcesandtools/tools-and-samples/hr-glossary/pages/labor-force.aspx" xr:uid="{FDB0E202-E4FF-D343-9B80-9C2ED4D0A90E}"/>
-    <hyperlink ref="L32" r:id="rId5" xr:uid="{6B35E6B0-1E56-484D-8667-A9AA2EF1C1CB}"/>
-    <hyperlink ref="L31" r:id="rId6" xr:uid="{DF8C0B88-B153-1941-B651-BB4D80930F76}"/>
+    <hyperlink ref="L108" r:id="rId1" display="https://www.shrm.org/resourcesandtools/tools-and-samples/hr-glossary/pages/soft-skills.aspx" xr:uid="{11470350-D5B9-3F44-99ED-2B7C2330DD6C}"/>
+    <hyperlink ref="L109" r:id="rId2" display="https://www.shrm.org/resourcesandtools/tools-and-samples/hr-glossary/pages/labor-force.aspx" xr:uid="{FDB0E202-E4FF-D343-9B80-9C2ED4D0A90E}"/>
+    <hyperlink ref="L32" r:id="rId3" xr:uid="{6B35E6B0-1E56-484D-8667-A9AA2EF1C1CB}"/>
+    <hyperlink ref="L31" r:id="rId4" xr:uid="{DF8C0B88-B153-1941-B651-BB4D80930F76}"/>
+    <hyperlink ref="L112" r:id="rId5" xr:uid="{2E37B1FA-FDF2-BA46-80C1-FF4AF8255844}"/>
+    <hyperlink ref="L111" r:id="rId6" xr:uid="{34BE0F78-FFFD-A144-985C-D0C5E823C0F1}"/>
+    <hyperlink ref="L97" r:id="rId7" xr:uid="{40BF0265-4014-9143-9B3E-2B8EF1AEA5E4}"/>
+    <hyperlink ref="L78" r:id="rId8" xr:uid="{4D95A307-7EC3-734C-A1C4-3021EF7F9594}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <legacyDrawing r:id="rId7"/>
+  <legacyDrawing r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -8888,7 +9032,7 @@
       </c>
       <c r="E4" s="1">
         <f t="shared" ref="E4" ca="1" si="1">RAND()</f>
-        <v>0.32776501485324028</v>
+        <v>0.64883151521817106</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" ref="F4" si="2">IF(ISNUMBER(SEARCH(" ",D4)), LEN(LEFT(D4,FIND(" ",D4)-1)), LEN(D4))</f>
@@ -8961,7 +9105,7 @@
       </c>
       <c r="E6" s="1">
         <f t="shared" ref="E6:E10" ca="1" si="7">RAND()</f>
-        <v>0.37688285326509752</v>
+        <v>0.71314650382480238</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" ref="F6:F10" si="8">IF(ISNUMBER(SEARCH(" ",D6)), LEN(LEFT(D6,FIND(" ",D6)-1)), LEN(D6))</f>
@@ -8999,7 +9143,7 @@
       </c>
       <c r="E7" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>0.1444383321554813</v>
+        <v>0.99010474522908865</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="8"/>
@@ -9037,7 +9181,7 @@
       </c>
       <c r="E8" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>0.52562583477735525</v>
+        <v>0.58081244058946602</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="8"/>
@@ -9075,7 +9219,7 @@
       </c>
       <c r="E9" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>0.43133505872805578</v>
+        <v>0.35234973862722874</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="8"/>
@@ -9113,7 +9257,7 @@
       </c>
       <c r="E10" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>0.70600445275247503</v>
+        <v>0.9016369889728908</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="8"/>
@@ -9151,7 +9295,7 @@
       </c>
       <c r="E12" s="1">
         <f t="shared" ref="E12:E61" ca="1" si="14">RAND()</f>
-        <v>0.28003540772897628</v>
+        <v>0.93413130856654059</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" ref="F12:F61" si="15">IF(ISNUMBER(SEARCH(" ",D12)), LEN(LEFT(D12,FIND(" ",D12)-1)), LEN(D12))</f>
@@ -9192,7 +9336,7 @@
       </c>
       <c r="E13" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.32713506699761741</v>
+        <v>0.55556401616923767</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="15"/>
@@ -9233,7 +9377,7 @@
       </c>
       <c r="E14" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.9881522933408512</v>
+        <v>0.86837259262157995</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="15"/>
@@ -9274,7 +9418,7 @@
       </c>
       <c r="E15" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.44399299057116137</v>
+        <v>0.23360170048270923</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="15"/>
@@ -9315,7 +9459,7 @@
       </c>
       <c r="E16" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.50135071563786526</v>
+        <v>1.4775302127376988E-2</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="15"/>
@@ -9353,7 +9497,7 @@
       </c>
       <c r="E17" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.66394606227989572</v>
+        <v>0.28024544879373403</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="15"/>
@@ -9394,7 +9538,7 @@
       </c>
       <c r="E18" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.10915662335958076</v>
+        <v>0.26946821836336132</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="15"/>
@@ -9432,7 +9576,7 @@
       </c>
       <c r="E19" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.4728936772004827</v>
+        <v>0.81254029830411734</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="15"/>
@@ -9473,7 +9617,7 @@
       </c>
       <c r="E20" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>2.2423093226320967E-2</v>
+        <v>0.36170155894361766</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="15"/>
@@ -9511,7 +9655,7 @@
       </c>
       <c r="E21" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.16993026034418701</v>
+        <v>0.33256326483003251</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="15"/>
@@ -9552,7 +9696,7 @@
       </c>
       <c r="E22" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.28393483594567515</v>
+        <v>0.96964780272331652</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="15"/>
@@ -9593,7 +9737,7 @@
       </c>
       <c r="E23" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.72124148252559195</v>
+        <v>0.62675830059633486</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="15"/>
@@ -9631,7 +9775,7 @@
       </c>
       <c r="E24" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.72923577942873818</v>
+        <v>0.81537958926928433</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" si="15"/>
@@ -9672,7 +9816,7 @@
       </c>
       <c r="E25" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.48894915744459766</v>
+        <v>0.40072168337201397</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" si="15"/>
@@ -9713,7 +9857,7 @@
       </c>
       <c r="E26" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.99988094903521663</v>
+        <v>0.66402311724103591</v>
       </c>
       <c r="F26" s="1">
         <f t="shared" si="15"/>
@@ -9754,7 +9898,7 @@
       </c>
       <c r="E27" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>1.821375549693649E-2</v>
+        <v>7.3872162732742552E-2</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" si="15"/>
@@ -9795,7 +9939,7 @@
       </c>
       <c r="E28" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>2.4430932561521401E-2</v>
+        <v>0.86979696928564032</v>
       </c>
       <c r="F28" s="1">
         <f t="shared" si="15"/>
@@ -9836,7 +9980,7 @@
       </c>
       <c r="E29" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.34398686617164087</v>
+        <v>0.61034707206853434</v>
       </c>
       <c r="F29" s="1">
         <f t="shared" si="15"/>
@@ -9874,7 +10018,7 @@
       </c>
       <c r="E30" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.26791865408595494</v>
+        <v>0.48887702083904794</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" si="15"/>
@@ -9915,7 +10059,7 @@
       </c>
       <c r="E31" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.66650487752753951</v>
+        <v>0.96356587784327552</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" si="15"/>
@@ -9956,7 +10100,7 @@
       </c>
       <c r="E32" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.33831329034028512</v>
+        <v>0.71148882953260528</v>
       </c>
       <c r="F32" s="1">
         <f t="shared" si="15"/>
@@ -9997,7 +10141,7 @@
       </c>
       <c r="E33" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.82953511550104142</v>
+        <v>0.42270766544553806</v>
       </c>
       <c r="F33" s="1">
         <f t="shared" si="15"/>
@@ -10035,7 +10179,7 @@
       </c>
       <c r="E34" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.2835206631401892</v>
+        <v>0.79404657902197162</v>
       </c>
       <c r="F34" s="1">
         <f t="shared" si="15"/>
@@ -10076,7 +10220,7 @@
       </c>
       <c r="E35" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.13233895591223233</v>
+        <v>0.110518112512487</v>
       </c>
       <c r="F35" s="1">
         <f t="shared" si="15"/>
@@ -10114,7 +10258,7 @@
       </c>
       <c r="E36" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>6.2921741078437288E-2</v>
+        <v>0.50650805362783113</v>
       </c>
       <c r="F36" s="1">
         <f t="shared" si="15"/>
@@ -10155,7 +10299,7 @@
       </c>
       <c r="E37" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.88089202997600435</v>
+        <v>8.7769898443983085E-2</v>
       </c>
       <c r="F37" s="1">
         <f t="shared" si="15"/>
@@ -10196,7 +10340,7 @@
       </c>
       <c r="E38" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.40461414187562716</v>
+        <v>0.93479207419272303</v>
       </c>
       <c r="F38" s="1">
         <f t="shared" si="15"/>
@@ -10237,7 +10381,7 @@
       </c>
       <c r="E39" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.71013453602102095</v>
+        <v>0.9291009526604922</v>
       </c>
       <c r="F39" s="1">
         <f t="shared" si="15"/>
@@ -10278,7 +10422,7 @@
       </c>
       <c r="E40" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.12584089244950758</v>
+        <v>0.69221249986713607</v>
       </c>
       <c r="F40" s="1">
         <f t="shared" si="15"/>
@@ -10319,7 +10463,7 @@
       </c>
       <c r="E41" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.3171108236796486</v>
+        <v>6.2676935792925437E-2</v>
       </c>
       <c r="F41" s="1">
         <f t="shared" si="15"/>
@@ -10360,7 +10504,7 @@
       </c>
       <c r="E42" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.28931057562067974</v>
+        <v>0.35070996944453292</v>
       </c>
       <c r="F42" s="1">
         <f t="shared" si="15"/>
@@ -10401,7 +10545,7 @@
       </c>
       <c r="E43" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.25739062299750937</v>
+        <v>0.47653808718212687</v>
       </c>
       <c r="F43" s="1">
         <f t="shared" si="15"/>
@@ -10439,7 +10583,7 @@
       </c>
       <c r="E44" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.79650735393367933</v>
+        <v>0.32848773215874416</v>
       </c>
       <c r="F44" s="1">
         <f t="shared" si="15"/>
@@ -10477,7 +10621,7 @@
       </c>
       <c r="E45" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.7311335194685542</v>
+        <v>0.54554721241726445</v>
       </c>
       <c r="F45" s="1">
         <f t="shared" si="15"/>
@@ -10518,7 +10662,7 @@
       </c>
       <c r="E46" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.99807063589427414</v>
+        <v>0.98461999037554981</v>
       </c>
       <c r="F46" s="1">
         <f t="shared" si="15"/>
@@ -10559,7 +10703,7 @@
       </c>
       <c r="E47" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.20885427809562662</v>
+        <v>0.92247104689689852</v>
       </c>
       <c r="F47" s="1">
         <f t="shared" si="15"/>
@@ -10597,7 +10741,7 @@
       </c>
       <c r="E48" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.59317085382178047</v>
+        <v>0.20834492719486519</v>
       </c>
       <c r="F48" s="1">
         <f t="shared" si="15"/>
@@ -10638,7 +10782,7 @@
       </c>
       <c r="E49" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.2415250321598984</v>
+        <v>0.87890581923009969</v>
       </c>
       <c r="F49" s="1">
         <f t="shared" si="15"/>
@@ -10676,7 +10820,7 @@
       </c>
       <c r="E50" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>5.240206192799779E-2</v>
+        <v>0.54089196575287657</v>
       </c>
       <c r="F50" s="1">
         <f t="shared" si="15"/>
@@ -10717,7 +10861,7 @@
       </c>
       <c r="E51" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>2.2229317293874784E-3</v>
+        <v>0.47443319526005134</v>
       </c>
       <c r="F51" s="1">
         <f t="shared" si="15"/>
@@ -10758,7 +10902,7 @@
       </c>
       <c r="E52" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.80766258464358909</v>
+        <v>0.27939175091858603</v>
       </c>
       <c r="F52" s="1">
         <f t="shared" si="15"/>
@@ -10796,7 +10940,7 @@
       </c>
       <c r="E53" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.77596583545720021</v>
+        <v>0.10683045359161991</v>
       </c>
       <c r="F53" s="1">
         <f t="shared" si="15"/>
@@ -10834,7 +10978,7 @@
       </c>
       <c r="E54" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.1900485096468062</v>
+        <v>0.36213498117804055</v>
       </c>
       <c r="F54" s="1">
         <f t="shared" si="15"/>
@@ -10875,7 +11019,7 @@
       </c>
       <c r="E55" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.72515740043062216</v>
+        <v>0.94503399049133197</v>
       </c>
       <c r="F55" s="1">
         <f t="shared" si="15"/>
@@ -10913,7 +11057,7 @@
       </c>
       <c r="E56" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.96514632038149895</v>
+        <v>3.6823394927069986E-2</v>
       </c>
       <c r="F56" s="1">
         <f t="shared" si="15"/>
@@ -10954,7 +11098,7 @@
       </c>
       <c r="E57" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.15656586514323545</v>
+        <v>0.81444010280715862</v>
       </c>
       <c r="F57" s="1">
         <f t="shared" si="15"/>
@@ -10995,7 +11139,7 @@
       </c>
       <c r="E58" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.8638700945725889</v>
+        <v>0.72613008044438088</v>
       </c>
       <c r="F58" s="1">
         <f t="shared" si="15"/>
@@ -11036,7 +11180,7 @@
       </c>
       <c r="E59" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.5042489003709274</v>
+        <v>0.55284167265390649</v>
       </c>
       <c r="F59" s="1">
         <f t="shared" si="15"/>
@@ -11077,7 +11221,7 @@
       </c>
       <c r="E60" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.87026254860177599</v>
+        <v>0.89442799876520551</v>
       </c>
       <c r="F60" s="1">
         <f t="shared" si="15"/>
@@ -11118,7 +11262,7 @@
       </c>
       <c r="E61" s="1">
         <f t="shared" ca="1" si="14"/>
-        <v>0.7765000574698353</v>
+        <v>0.20626574791795593</v>
       </c>
       <c r="F61" s="1">
         <f t="shared" si="15"/>
@@ -11145,7 +11289,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H6">
-    <cfRule type="containsText" dxfId="115" priority="123" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="97" priority="123" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H6)))</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="126">
@@ -11153,22 +11297,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="114" priority="124" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="96" priority="124" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="containsText" dxfId="113" priority="127" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="95" priority="127" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="112" priority="125" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="94" priority="125" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="containsText" dxfId="111" priority="118" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="93" priority="118" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H4)))</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="121">
@@ -11176,22 +11320,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="110" priority="119" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="92" priority="119" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4">
-    <cfRule type="containsText" dxfId="109" priority="122" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="91" priority="122" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="cellIs" dxfId="108" priority="120" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="90" priority="120" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="containsText" dxfId="107" priority="113" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="89" priority="113" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H7)))</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="116">
@@ -11199,22 +11343,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="cellIs" dxfId="106" priority="114" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="88" priority="114" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="containsText" dxfId="105" priority="117" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="87" priority="117" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="104" priority="115" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="86" priority="115" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H14">
-    <cfRule type="containsText" dxfId="103" priority="108" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="85" priority="108" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H12)))</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="111">
@@ -11222,22 +11366,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F14">
-    <cfRule type="cellIs" dxfId="102" priority="109" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="84" priority="109" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12:K14">
-    <cfRule type="containsText" dxfId="101" priority="112" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="83" priority="112" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G14">
-    <cfRule type="cellIs" dxfId="100" priority="110" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="82" priority="110" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="containsText" dxfId="99" priority="103" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="81" priority="103" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H15)))</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="106">
@@ -11245,22 +11389,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="cellIs" dxfId="98" priority="104" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="80" priority="104" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="containsText" dxfId="97" priority="107" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="79" priority="107" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15">
-    <cfRule type="cellIs" dxfId="96" priority="105" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="78" priority="105" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:H17">
-    <cfRule type="containsText" dxfId="95" priority="98" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="77" priority="98" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H16)))</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="101">
@@ -11268,22 +11412,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:F17">
-    <cfRule type="cellIs" dxfId="94" priority="99" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="76" priority="99" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16:K17">
-    <cfRule type="containsText" dxfId="93" priority="102" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="75" priority="102" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16:G17">
-    <cfRule type="cellIs" dxfId="92" priority="100" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="74" priority="100" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:H19">
-    <cfRule type="containsText" dxfId="91" priority="93" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="73" priority="93" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H18)))</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="96">
@@ -11291,22 +11435,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18:F19">
-    <cfRule type="cellIs" dxfId="90" priority="94" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="94" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18:K19">
-    <cfRule type="containsText" dxfId="89" priority="97" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="71" priority="97" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18:G19">
-    <cfRule type="cellIs" dxfId="88" priority="95" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="70" priority="95" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20">
-    <cfRule type="containsText" dxfId="87" priority="88" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="69" priority="88" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H20)))</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="91">
@@ -11314,22 +11458,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="cellIs" dxfId="86" priority="89" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="89" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="containsText" dxfId="85" priority="92" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="67" priority="92" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20">
-    <cfRule type="cellIs" dxfId="84" priority="90" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="66" priority="90" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21:H31">
-    <cfRule type="containsText" dxfId="83" priority="73" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="65" priority="73" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H21)))</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="76">
@@ -11337,22 +11481,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21:F31">
-    <cfRule type="cellIs" dxfId="82" priority="74" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="64" priority="74" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21:K31">
-    <cfRule type="containsText" dxfId="81" priority="77" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="63" priority="77" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21:G31">
-    <cfRule type="cellIs" dxfId="80" priority="75" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="75" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="containsText" dxfId="79" priority="68" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="61" priority="68" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H32)))</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="71">
@@ -11360,22 +11504,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32">
-    <cfRule type="cellIs" dxfId="78" priority="69" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="60" priority="69" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="containsText" dxfId="77" priority="72" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="59" priority="72" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32">
-    <cfRule type="cellIs" dxfId="76" priority="70" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="70" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:H34">
-    <cfRule type="containsText" dxfId="75" priority="63" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="57" priority="63" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H33)))</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="66">
@@ -11383,22 +11527,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F33:F34">
-    <cfRule type="cellIs" dxfId="74" priority="64" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="56" priority="64" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K33:K34">
-    <cfRule type="containsText" dxfId="73" priority="67" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="55" priority="67" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33:G34">
-    <cfRule type="cellIs" dxfId="72" priority="65" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="65" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35:H36">
-    <cfRule type="containsText" dxfId="71" priority="58" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="53" priority="58" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H35)))</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="61">
@@ -11406,22 +11550,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35:F36">
-    <cfRule type="cellIs" dxfId="70" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="52" priority="59" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35:K36">
-    <cfRule type="containsText" dxfId="69" priority="62" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="51" priority="62" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35:G36">
-    <cfRule type="cellIs" dxfId="68" priority="60" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="60" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="containsText" dxfId="67" priority="53" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="49" priority="53" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H37)))</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="56">
@@ -11429,22 +11573,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F37">
-    <cfRule type="cellIs" dxfId="66" priority="54" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="48" priority="54" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K37">
-    <cfRule type="containsText" dxfId="65" priority="57" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="47" priority="57" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37">
-    <cfRule type="cellIs" dxfId="64" priority="55" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="55" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38:H40">
-    <cfRule type="containsText" dxfId="63" priority="48" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="45" priority="48" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H38)))</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="51">
@@ -11452,22 +11596,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F38:F40">
-    <cfRule type="cellIs" dxfId="62" priority="49" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="49" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K38:K40">
-    <cfRule type="containsText" dxfId="61" priority="52" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="43" priority="52" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38:G40">
-    <cfRule type="cellIs" dxfId="60" priority="50" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="50" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41:H56">
-    <cfRule type="containsText" dxfId="59" priority="43" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="41" priority="43" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H41)))</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="46">
@@ -11475,22 +11619,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F41:F56">
-    <cfRule type="cellIs" dxfId="58" priority="44" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="44" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K41:K56">
-    <cfRule type="containsText" dxfId="57" priority="47" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="39" priority="47" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G41:G56">
-    <cfRule type="cellIs" dxfId="56" priority="45" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="45" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="containsText" dxfId="55" priority="38" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H8)))</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="41">
@@ -11498,27 +11642,27 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="54" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="39" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="containsText" dxfId="53" priority="42" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="35" priority="42" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="52" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="40" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsBlanks" dxfId="51" priority="37">
+    <cfRule type="containsBlanks" dxfId="33" priority="37">
       <formula>LEN(TRIM(D8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="containsText" dxfId="50" priority="32" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="32" priority="32" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H9)))</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="35">
@@ -11526,27 +11670,27 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="49" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="33" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="containsText" dxfId="48" priority="36" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="30" priority="36" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="cellIs" dxfId="47" priority="34" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="34" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="containsBlanks" dxfId="46" priority="31">
+    <cfRule type="containsBlanks" dxfId="28" priority="31">
       <formula>LEN(TRIM(D9))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="containsText" dxfId="45" priority="26" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="27" priority="26" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H10)))</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="29">
@@ -11554,27 +11698,27 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="cellIs" dxfId="44" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="27" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="containsText" dxfId="43" priority="30" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="cellIs" dxfId="42" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="28" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="containsBlanks" dxfId="41" priority="25">
+    <cfRule type="containsBlanks" dxfId="23" priority="25">
       <formula>LEN(TRIM(D10))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57">
-    <cfRule type="containsText" dxfId="40" priority="20" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H57)))</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="23">
@@ -11582,27 +11726,27 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57">
-    <cfRule type="cellIs" dxfId="39" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K57">
-    <cfRule type="containsText" dxfId="38" priority="24" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G57">
-    <cfRule type="cellIs" dxfId="37" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="22" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D57">
-    <cfRule type="containsBlanks" dxfId="36" priority="19">
+    <cfRule type="containsBlanks" dxfId="18" priority="19">
       <formula>LEN(TRIM(D57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H58">
-    <cfRule type="containsText" dxfId="35" priority="14" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="17" priority="14" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H58)))</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="17">
@@ -11610,27 +11754,27 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F58">
-    <cfRule type="cellIs" dxfId="34" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K58">
-    <cfRule type="containsText" dxfId="33" priority="18" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G58">
-    <cfRule type="cellIs" dxfId="32" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D58">
-    <cfRule type="containsBlanks" dxfId="31" priority="13">
+    <cfRule type="containsBlanks" dxfId="13" priority="13">
       <formula>LEN(TRIM(D58))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59">
-    <cfRule type="containsText" dxfId="30" priority="9" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H59)))</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="12">
@@ -11638,27 +11782,27 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F59">
-    <cfRule type="cellIs" dxfId="29" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G59">
-    <cfRule type="cellIs" dxfId="28" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D59">
-    <cfRule type="containsBlanks" dxfId="27" priority="8">
+    <cfRule type="containsBlanks" dxfId="9" priority="8">
       <formula>LEN(TRIM(D59))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K59">
-    <cfRule type="containsText" dxfId="26" priority="7" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H60:H61">
-    <cfRule type="containsText" dxfId="25" priority="3" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",H60)))</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="6">
@@ -11666,22 +11810,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F60:F61">
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G60:G61">
-    <cfRule type="cellIs" dxfId="23" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D60:D61">
-    <cfRule type="containsBlanks" dxfId="22" priority="2">
+    <cfRule type="containsBlanks" dxfId="4" priority="2">
       <formula>LEN(TRIM(D60))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K60:K61">
-    <cfRule type="containsText" dxfId="21" priority="1" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",K60)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>